<commit_message>
Add basic auth framework
</commit_message>
<xml_diff>
--- a/gourmet/restaurant_list/sophia_test_data.xlsx
+++ b/gourmet/restaurant_list/sophia_test_data.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1008" uniqueCount="611">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1002" uniqueCount="611">
   <si>
     <t>Sat   8:00 AM- 3:00 PM</t>
   </si>
@@ -1313,9 +1313,6 @@
     <t>Zazie*</t>
   </si>
   <si>
-    <t>Dottie’s True Blue Café*</t>
-  </si>
-  <si>
     <t xml:space="preserve">*Open for weekday breakfast </t>
   </si>
   <si>
@@ -2211,6 +2208,9 @@
   </si>
   <si>
     <t>AQ Restaurant &amp; Bar</t>
+  </si>
+  <si>
+    <t>Dottie's True Blue Café*</t>
   </si>
 </sst>
 </file>
@@ -2822,7 +2822,7 @@
   <dimension ref="A1:K251"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -2842,22 +2842,22 @@
   <sheetData>
     <row r="1" spans="1:11" ht="45" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>80</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="F1" s="18" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="G1" s="8" t="s">
         <v>79</v>
@@ -2867,22 +2867,22 @@
       </c>
       <c r="I1" s="43"/>
       <c r="J1" s="43" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="K1" s="43"/>
     </row>
     <row r="2" spans="1:11" s="17" customFormat="1" ht="12.75" customHeight="1">
       <c r="A2" s="33" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D2" s="33" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E2" s="6">
         <v>90</v>
@@ -2900,7 +2900,7 @@
         <v>13</v>
       </c>
       <c r="J2" s="11" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="K2"/>
     </row>
@@ -2909,13 +2909,13 @@
         <v>110</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D3" s="33" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E3" s="6">
         <v>90</v>
@@ -2937,16 +2937,16 @@
     </row>
     <row r="4" spans="1:11" s="17" customFormat="1" ht="12.75" customHeight="1">
       <c r="A4" s="33" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D4" s="33" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E4" s="11">
         <v>90</v>
@@ -2973,10 +2973,10 @@
         <v>26</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D5" s="33" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E5" s="11">
         <v>95</v>
@@ -2988,7 +2988,7 @@
         <v>314</v>
       </c>
       <c r="H5" s="11" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="I5" s="16" t="s">
         <v>27</v>
@@ -3004,10 +3004,10 @@
         <v>19</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D6" s="33" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E6" s="11">
         <v>95</v>
@@ -3016,7 +3016,7 @@
         <v>5</v>
       </c>
       <c r="G6" s="15" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="H6" s="16" t="s">
         <v>20</v>
@@ -3035,10 +3035,10 @@
         <v>248</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D7" s="33" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E7" s="11">
         <v>95</v>
@@ -3060,16 +3060,16 @@
     </row>
     <row r="8" spans="1:11" ht="12.75" customHeight="1">
       <c r="A8" s="33" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="B8" s="15" t="s">
         <v>259</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D8" s="33" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E8" s="11">
         <v>90</v>
@@ -3091,16 +3091,16 @@
     </row>
     <row r="9" spans="1:11" s="1" customFormat="1" ht="12.75" customHeight="1">
       <c r="A9" s="40" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D9" s="40" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="E9" s="39">
         <v>95</v>
@@ -3109,13 +3109,13 @@
         <v>4</v>
       </c>
       <c r="G9" s="15" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="H9" s="10" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="J9" s="34"/>
     </row>
@@ -3127,10 +3127,10 @@
         <v>313</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D10" s="33" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E10" s="11">
         <v>85</v>
@@ -3139,13 +3139,13 @@
         <v>8</v>
       </c>
       <c r="G10" s="15" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="H10" s="11" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="J10" s="11"/>
       <c r="K10" s="17"/>
@@ -3158,10 +3158,10 @@
         <v>50</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D11" s="33" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E11" s="11">
         <v>85</v>
@@ -3170,10 +3170,10 @@
         <v>10</v>
       </c>
       <c r="G11" s="15" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="H11" s="11" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="I11" s="16" t="s">
         <v>1</v>
@@ -3188,10 +3188,10 @@
         <v>14</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D12" s="33" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E12" s="11">
         <v>85</v>
@@ -3200,7 +3200,7 @@
         <v>11</v>
       </c>
       <c r="G12" s="15" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="H12" s="16" t="s">
         <v>15</v>
@@ -3218,10 +3218,10 @@
         <v>39</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="E13" s="11">
         <v>92</v>
@@ -3233,7 +3233,7 @@
         <v>241</v>
       </c>
       <c r="H13" s="11" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="I13" s="16" t="s">
         <v>242</v>
@@ -3242,16 +3242,16 @@
     </row>
     <row r="14" spans="1:11" s="17" customFormat="1" ht="12.75" customHeight="1">
       <c r="A14" s="33" t="s">
+        <v>348</v>
+      </c>
+      <c r="B14" s="17" t="s">
         <v>349</v>
       </c>
-      <c r="B14" s="17" t="s">
-        <v>350</v>
-      </c>
       <c r="C14" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D14" s="17" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="E14" s="11">
         <v>85</v>
@@ -3260,16 +3260,16 @@
         <v>13</v>
       </c>
       <c r="G14" s="15" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="H14" s="16" t="s">
+        <v>384</v>
+      </c>
+      <c r="I14" s="16" t="s">
         <v>385</v>
       </c>
-      <c r="I14" s="16" t="s">
-        <v>386</v>
-      </c>
       <c r="J14" s="11" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="15" spans="1:11" s="17" customFormat="1" ht="12.75" customHeight="1">
@@ -3280,10 +3280,10 @@
         <v>320</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D15" s="33" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E15" s="6">
         <v>85</v>
@@ -3295,7 +3295,7 @@
         <v>329</v>
       </c>
       <c r="H15" s="11" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="I15" s="2" t="s">
         <v>1</v>
@@ -3311,10 +3311,10 @@
         <v>213</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="E16" s="6">
         <v>85</v>
@@ -3331,16 +3331,16 @@
     </row>
     <row r="17" spans="1:11" ht="12.75" customHeight="1">
       <c r="A17" s="4" t="s">
-        <v>331</v>
+        <v>610</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>217</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="E17" s="6">
         <v>80</v>
@@ -3355,21 +3355,21 @@
         <v>8</v>
       </c>
       <c r="J17" s="6" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="12.75" customHeight="1">
       <c r="A18" s="33" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>2</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="E18" s="6">
         <v>80</v>
@@ -3384,7 +3384,7 @@
         <v>4</v>
       </c>
       <c r="J18" s="11" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="19" spans="1:11" s="17" customFormat="1" ht="12.75" customHeight="1">
@@ -3395,10 +3395,10 @@
         <v>28</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="E19" s="11">
         <v>80</v>
@@ -3423,10 +3423,10 @@
         <v>24</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D20" s="33" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E20" s="11">
         <v>80</v>
@@ -3443,18 +3443,18 @@
       </c>
       <c r="J20" s="11"/>
     </row>
-    <row r="21" spans="1:11" s="17" customFormat="1" ht="12.75" customHeight="1">
+    <row r="21" spans="1:11" s="17" customFormat="1" ht="11" customHeight="1">
       <c r="A21" s="33" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>216</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="E21" s="6">
         <v>75</v>
@@ -3470,22 +3470,22 @@
         <v>1</v>
       </c>
       <c r="J21" s="11" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="K21"/>
     </row>
     <row r="22" spans="1:11" s="17" customFormat="1" ht="12.75" customHeight="1">
       <c r="A22" s="33" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>218</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D22" s="33" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E22" s="6">
         <v>70</v>
@@ -3501,62 +3501,62 @@
         <v>10</v>
       </c>
       <c r="J22" s="11" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="K22"/>
     </row>
     <row r="23" spans="1:11" s="17" customFormat="1" ht="12.75" customHeight="1">
       <c r="A23" s="12" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="B23" s="12" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D23" s="35" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="E23" s="6"/>
       <c r="F23" s="6"/>
       <c r="G23" s="12" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="H23" s="3" t="s">
         <v>3</v>
       </c>
       <c r="I23" s="3" t="s">
+        <v>497</v>
+      </c>
+      <c r="J23" s="10" t="s">
         <v>498</v>
-      </c>
-      <c r="J23" s="10" t="s">
-        <v>499</v>
       </c>
       <c r="K23"/>
     </row>
     <row r="24" spans="1:11" s="25" customFormat="1" ht="12.75" customHeight="1">
       <c r="A24" s="35" t="s">
+        <v>381</v>
+      </c>
+      <c r="B24" s="25" t="s">
         <v>382</v>
       </c>
-      <c r="B24" s="25" t="s">
-        <v>383</v>
-      </c>
       <c r="C24" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D24" s="25" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="E24" s="10"/>
       <c r="F24" s="10"/>
       <c r="G24" s="12" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="H24" s="3" t="s">
+        <v>386</v>
+      </c>
+      <c r="I24" s="3" t="s">
         <v>387</v>
-      </c>
-      <c r="I24" s="3" t="s">
-        <v>388</v>
       </c>
       <c r="J24" s="10"/>
     </row>
@@ -3565,18 +3565,18 @@
         <v>330</v>
       </c>
       <c r="B25" s="12" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D25" s="12" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="E25" s="10"/>
       <c r="F25" s="10"/>
       <c r="G25" s="12" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="H25" s="3" t="s">
         <v>31</v>
@@ -3585,16 +3585,16 @@
         <v>32</v>
       </c>
       <c r="J25" s="10" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="26" spans="1:11" ht="12.75" customHeight="1">
       <c r="A26" s="15" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B26" s="12"/>
       <c r="C26" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D26" s="12"/>
       <c r="E26" s="10"/>
@@ -3607,7 +3607,7 @@
       <c r="A27" s="15"/>
       <c r="B27" s="12"/>
       <c r="C27" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D27" s="12"/>
       <c r="E27" s="10"/>
@@ -3618,12 +3618,10 @@
     </row>
     <row r="28" spans="1:11" s="17" customFormat="1" ht="12.75" customHeight="1">
       <c r="A28" s="38" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="B28" s="15"/>
-      <c r="C28" s="4" t="s">
-        <v>608</v>
-      </c>
+      <c r="C28" s="4"/>
       <c r="D28" s="15"/>
       <c r="E28" s="11"/>
       <c r="F28" s="11"/>
@@ -3634,11 +3632,11 @@
     </row>
     <row r="29" spans="1:11" ht="12.75" customHeight="1">
       <c r="A29" s="15" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="B29" s="12"/>
       <c r="C29" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D29" s="12"/>
       <c r="E29" s="10"/>
@@ -3649,11 +3647,11 @@
     </row>
     <row r="30" spans="1:11" ht="12.75" customHeight="1">
       <c r="A30" s="15" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="B30" s="12"/>
       <c r="C30" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D30" s="12"/>
       <c r="E30" s="10"/>
@@ -3664,11 +3662,11 @@
     </row>
     <row r="31" spans="1:11" ht="12.75" customHeight="1">
       <c r="A31" s="15" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="B31" s="12"/>
       <c r="C31" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D31" s="12"/>
       <c r="E31" s="10"/>
@@ -3679,11 +3677,11 @@
     </row>
     <row r="32" spans="1:11" ht="12.75" customHeight="1">
       <c r="A32" s="15" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="B32" s="12"/>
       <c r="C32" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D32" s="12"/>
       <c r="E32" s="10"/>
@@ -3694,11 +3692,11 @@
     </row>
     <row r="33" spans="1:10" ht="12.75" customHeight="1">
       <c r="A33" s="15" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="B33" s="12"/>
       <c r="C33" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D33" s="12"/>
       <c r="E33" s="10"/>
@@ -3709,11 +3707,11 @@
     </row>
     <row r="34" spans="1:10" ht="12.75" customHeight="1">
       <c r="A34" s="15" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="B34" s="12"/>
       <c r="C34" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D34" s="12"/>
       <c r="E34" s="10"/>
@@ -3724,11 +3722,11 @@
     </row>
     <row r="35" spans="1:10" ht="12.75" customHeight="1">
       <c r="A35" s="15" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="B35" s="12"/>
       <c r="C35" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D35" s="12"/>
       <c r="E35" s="10"/>
@@ -3739,11 +3737,11 @@
     </row>
     <row r="36" spans="1:10" ht="12.75" customHeight="1">
       <c r="A36" s="15" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="B36" s="12"/>
       <c r="C36" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D36" s="12"/>
       <c r="E36" s="10"/>
@@ -3754,11 +3752,11 @@
     </row>
     <row r="37" spans="1:10" ht="12.75" customHeight="1">
       <c r="A37" s="15" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="B37" s="12"/>
       <c r="C37" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D37" s="12"/>
       <c r="E37" s="10"/>
@@ -3769,11 +3767,11 @@
     </row>
     <row r="38" spans="1:10" ht="12.75" customHeight="1">
       <c r="A38" s="15" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="B38" s="12"/>
       <c r="C38" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D38" s="12"/>
       <c r="E38" s="10"/>
@@ -3784,11 +3782,11 @@
     </row>
     <row r="39" spans="1:10" ht="12.75" customHeight="1">
       <c r="A39" s="15" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="B39" s="12"/>
       <c r="C39" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D39" s="12"/>
       <c r="E39" s="10"/>
@@ -3799,11 +3797,11 @@
     </row>
     <row r="40" spans="1:10" ht="12.75" customHeight="1">
       <c r="A40" s="15" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="B40" s="12"/>
       <c r="C40" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D40" s="12"/>
       <c r="E40" s="10"/>
@@ -3814,11 +3812,11 @@
     </row>
     <row r="41" spans="1:10" ht="12.75" customHeight="1">
       <c r="A41" s="12" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="B41" s="12"/>
       <c r="C41" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D41" s="12"/>
       <c r="E41" s="10"/>
@@ -3829,11 +3827,11 @@
     </row>
     <row r="42" spans="1:10" ht="12.75" customHeight="1">
       <c r="A42" s="12" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="B42" s="12"/>
       <c r="C42" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D42" s="12"/>
       <c r="E42" s="10"/>
@@ -3846,7 +3844,7 @@
       <c r="A43" s="12"/>
       <c r="B43" s="12"/>
       <c r="C43" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D43" s="12"/>
       <c r="E43" s="10"/>
@@ -3860,9 +3858,6 @@
         <v>33</v>
       </c>
       <c r="B44" s="5"/>
-      <c r="C44" s="4" t="s">
-        <v>608</v>
-      </c>
       <c r="D44" s="5"/>
       <c r="E44" s="7"/>
       <c r="F44" s="14"/>
@@ -3872,13 +3867,13 @@
     </row>
     <row r="45" spans="1:10" ht="12.75" customHeight="1">
       <c r="A45" s="33" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="B45" s="4" t="s">
         <v>34</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="E45" s="11">
         <v>95</v>
@@ -3887,7 +3882,7 @@
         <v>1</v>
       </c>
       <c r="G45" s="4" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="H45" s="6"/>
       <c r="I45" s="6"/>
@@ -3897,10 +3892,10 @@
         <v>244</v>
       </c>
       <c r="B46" s="15" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D46" s="15"/>
       <c r="E46" s="11">
@@ -3910,20 +3905,20 @@
         <v>2</v>
       </c>
       <c r="G46" s="4" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="H46" s="6"/>
       <c r="I46" s="6"/>
     </row>
     <row r="47" spans="1:10" ht="12.75" customHeight="1">
       <c r="A47" s="33" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B47" s="4" t="s">
         <v>220</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="E47" s="6">
         <v>90</v>
@@ -3932,20 +3927,20 @@
         <v>3</v>
       </c>
       <c r="G47" s="4" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="H47" s="6"/>
       <c r="I47" s="6"/>
     </row>
     <row r="48" spans="1:10" s="17" customFormat="1" ht="12.75" customHeight="1">
       <c r="A48" s="33" t="s">
+        <v>504</v>
+      </c>
+      <c r="B48" s="15" t="s">
         <v>505</v>
       </c>
-      <c r="B48" s="15" t="s">
-        <v>506</v>
-      </c>
       <c r="C48" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D48" s="15"/>
       <c r="E48" s="11">
@@ -3955,7 +3950,7 @@
         <v>4</v>
       </c>
       <c r="G48" s="15" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="H48" s="11"/>
       <c r="I48" s="11"/>
@@ -3969,7 +3964,7 @@
         <v>39</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="E49" s="6">
         <v>85</v>
@@ -3986,7 +3981,7 @@
         <v>222</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="E50" s="6">
         <v>80</v>
@@ -4005,7 +4000,7 @@
         <v>221</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="E51" s="6">
         <v>80</v>
@@ -4022,7 +4017,7 @@
         <v>50</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D52" s="15"/>
       <c r="G52" s="4"/>
@@ -4031,73 +4026,73 @@
     </row>
     <row r="53" spans="1:11" ht="12.75" customHeight="1">
       <c r="A53" s="33" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="B53" s="15" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D53" s="15"/>
       <c r="E53" s="6">
         <v>60</v>
       </c>
       <c r="G53" s="4" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="H53" s="6"/>
       <c r="I53" s="6"/>
     </row>
     <row r="54" spans="1:11" ht="12.75" customHeight="1">
       <c r="A54" s="40" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="B54" s="41" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D54" s="12"/>
       <c r="E54" s="6">
         <v>75</v>
       </c>
       <c r="G54" s="4" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="H54" s="6"/>
       <c r="I54" s="6"/>
     </row>
     <row r="55" spans="1:11" ht="12.75" customHeight="1">
       <c r="A55" s="40" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="B55" s="42" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D55" s="12"/>
       <c r="E55" s="6">
         <v>80</v>
       </c>
       <c r="G55" s="4" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="H55" s="6"/>
       <c r="I55" s="6"/>
     </row>
     <row r="56" spans="1:11" ht="12.75" customHeight="1">
       <c r="A56" s="40" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="B56" s="15" t="s">
         <v>35</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D56" s="15"/>
       <c r="E56" s="11">
@@ -4105,20 +4100,20 @@
       </c>
       <c r="F56" s="10"/>
       <c r="G56" s="4" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="H56" s="6"/>
       <c r="I56" s="6"/>
     </row>
     <row r="57" spans="1:11" ht="12.75" customHeight="1">
       <c r="A57" s="40" t="s">
+        <v>595</v>
+      </c>
+      <c r="B57" s="15" t="s">
         <v>596</v>
       </c>
-      <c r="B57" s="15" t="s">
-        <v>597</v>
-      </c>
       <c r="C57" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D57" s="12"/>
       <c r="E57" s="11">
@@ -4126,20 +4121,20 @@
       </c>
       <c r="F57" s="10"/>
       <c r="G57" s="4" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="H57" s="6"/>
       <c r="I57" s="6"/>
     </row>
     <row r="58" spans="1:11" ht="12.75" customHeight="1">
       <c r="A58" s="35" t="s">
+        <v>591</v>
+      </c>
+      <c r="B58" s="12" t="s">
         <v>592</v>
       </c>
-      <c r="B58" s="12" t="s">
-        <v>593</v>
-      </c>
       <c r="C58" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D58" s="12"/>
       <c r="E58" s="10"/>
@@ -4150,13 +4145,13 @@
     </row>
     <row r="59" spans="1:11" ht="12.75" customHeight="1">
       <c r="A59" s="35" t="s">
+        <v>593</v>
+      </c>
+      <c r="B59" s="12" t="s">
         <v>594</v>
       </c>
-      <c r="B59" s="12" t="s">
-        <v>595</v>
-      </c>
       <c r="C59" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D59" s="12"/>
       <c r="E59" s="10"/>
@@ -4167,13 +4162,13 @@
     </row>
     <row r="60" spans="1:11" s="25" customFormat="1" ht="12.75" customHeight="1">
       <c r="A60" s="35" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B60" s="12" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D60" s="12"/>
       <c r="E60" s="10"/>
@@ -4187,7 +4182,7 @@
       <c r="A61" s="35"/>
       <c r="B61" s="12"/>
       <c r="C61" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D61" s="12"/>
       <c r="E61" s="10"/>
@@ -4202,9 +4197,7 @@
         <v>36</v>
       </c>
       <c r="B62" s="3"/>
-      <c r="C62" s="4" t="s">
-        <v>608</v>
-      </c>
+      <c r="C62" s="4"/>
       <c r="D62" s="3"/>
       <c r="E62" s="10"/>
       <c r="F62" s="10"/>
@@ -4221,7 +4214,7 @@
         <v>78</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="E63" s="11">
         <v>90</v>
@@ -4240,10 +4233,10 @@
         <v>255</v>
       </c>
       <c r="B64" s="15" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D64" s="15"/>
       <c r="E64" s="11">
@@ -4253,7 +4246,7 @@
         <v>4</v>
       </c>
       <c r="G64" s="15" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="H64" s="11"/>
       <c r="I64" s="11"/>
@@ -4268,7 +4261,7 @@
         <v>39</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="E65" s="11">
         <v>85</v>
@@ -4290,7 +4283,7 @@
         <v>238</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D66" s="15"/>
       <c r="E66" s="11">
@@ -4300,7 +4293,7 @@
         <v>2</v>
       </c>
       <c r="G66" s="15" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="H66" s="11"/>
       <c r="I66" s="11"/>
@@ -4315,17 +4308,17 @@
         <v>316</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D67" s="15"/>
       <c r="E67" s="11">
         <v>83</v>
       </c>
       <c r="F67" s="11" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="G67" s="15" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="H67" s="11"/>
       <c r="I67" s="11"/>
@@ -4333,13 +4326,13 @@
     </row>
     <row r="68" spans="1:11" s="17" customFormat="1" ht="12.75" customHeight="1">
       <c r="A68" s="15" t="s">
+        <v>371</v>
+      </c>
+      <c r="B68" s="15" t="s">
         <v>372</v>
       </c>
-      <c r="B68" s="15" t="s">
-        <v>373</v>
-      </c>
       <c r="C68" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D68" s="15"/>
       <c r="E68" s="11">
@@ -4347,7 +4340,7 @@
       </c>
       <c r="F68" s="11"/>
       <c r="G68" s="15" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="H68" s="11"/>
       <c r="I68" s="11"/>
@@ -4358,10 +4351,10 @@
         <v>94</v>
       </c>
       <c r="B69" s="15" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D69" s="15"/>
       <c r="E69" s="11">
@@ -4371,7 +4364,7 @@
         <v>5</v>
       </c>
       <c r="G69" s="15" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="H69" s="11"/>
       <c r="I69" s="11"/>
@@ -4386,7 +4379,7 @@
         <v>37</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D70" s="4"/>
       <c r="E70" s="11">
@@ -4405,13 +4398,13 @@
     </row>
     <row r="71" spans="1:11" s="17" customFormat="1" ht="12.75" customHeight="1">
       <c r="A71" s="15" t="s">
+        <v>367</v>
+      </c>
+      <c r="B71" s="15" t="s">
         <v>368</v>
       </c>
-      <c r="B71" s="15" t="s">
-        <v>369</v>
-      </c>
       <c r="C71" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D71" s="15"/>
       <c r="E71" s="11">
@@ -4421,7 +4414,7 @@
         <v>6</v>
       </c>
       <c r="G71" s="15" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="H71" s="11"/>
       <c r="I71" s="11"/>
@@ -4435,7 +4428,7 @@
         <v>40</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D72" s="4"/>
       <c r="E72" s="11">
@@ -4445,7 +4438,7 @@
         <v>8</v>
       </c>
       <c r="G72" s="4" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="H72" s="6"/>
       <c r="I72" s="6"/>
@@ -4460,7 +4453,7 @@
         <v>231</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D73" s="15"/>
       <c r="E73" s="11">
@@ -4468,7 +4461,7 @@
       </c>
       <c r="F73" s="11"/>
       <c r="G73" s="15" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="H73" s="11"/>
       <c r="I73" s="11"/>
@@ -4483,7 +4476,7 @@
         <v>38</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="E74" s="11">
         <v>65</v>
@@ -4505,7 +4498,7 @@
         <v>44</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D75" s="12"/>
       <c r="E75" s="10"/>
@@ -4524,7 +4517,7 @@
         <v>42</v>
       </c>
       <c r="C76" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D76" s="12"/>
       <c r="E76" s="10"/>
@@ -4541,7 +4534,7 @@
         <v>41</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D77" s="12"/>
       <c r="E77" s="10"/>
@@ -4560,7 +4553,7 @@
         <v>43</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D78" s="12"/>
       <c r="E78" s="10"/>
@@ -4571,7 +4564,7 @@
     </row>
     <row r="79" spans="1:11" ht="12.75" customHeight="1">
       <c r="C79" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="G79" s="4"/>
       <c r="H79" s="6"/>
@@ -4579,20 +4572,17 @@
     </row>
     <row r="80" spans="1:11" ht="12.75" customHeight="1">
       <c r="A80" s="1" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="B80" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="C80" s="4" t="s">
-        <v>608</v>
-      </c>
       <c r="D80" s="5"/>
       <c r="E80" s="9" t="s">
+        <v>601</v>
+      </c>
+      <c r="F80" s="9" t="s">
         <v>602</v>
-      </c>
-      <c r="F80" s="9" t="s">
-        <v>603</v>
       </c>
       <c r="G80" s="5" t="s">
         <v>269</v>
@@ -4610,7 +4600,7 @@
         <v>53</v>
       </c>
       <c r="C81" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D81" s="40" t="s">
         <v>110</v>
@@ -4622,7 +4612,7 @@
         <v>1</v>
       </c>
       <c r="G81" s="15" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="H81" s="15"/>
       <c r="I81" s="11"/>
@@ -4631,16 +4621,16 @@
     </row>
     <row r="82" spans="1:11" s="4" customFormat="1" ht="12.75" customHeight="1">
       <c r="A82" s="33" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="B82" s="15" t="s">
         <v>239</v>
       </c>
       <c r="C82" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D82" s="33" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E82" s="11">
         <v>90</v>
@@ -4664,10 +4654,10 @@
         <v>209</v>
       </c>
       <c r="C83" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D83" s="33" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E83" s="6">
         <v>85</v>
@@ -4676,7 +4666,7 @@
         <v>3</v>
       </c>
       <c r="G83" s="4" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="H83" s="4"/>
       <c r="I83" s="6"/>
@@ -4691,10 +4681,10 @@
         <v>214</v>
       </c>
       <c r="C84" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D84" s="33" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E84" s="6">
         <v>90</v>
@@ -4718,36 +4708,36 @@
         <v>258</v>
       </c>
       <c r="C85" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D85" s="40" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E85" s="11">
         <v>90</v>
       </c>
       <c r="F85" s="10"/>
       <c r="G85" s="15" t="s">
+        <v>551</v>
+      </c>
+      <c r="H85" s="13" t="s">
         <v>552</v>
-      </c>
-      <c r="H85" s="13" t="s">
-        <v>553</v>
       </c>
       <c r="I85" s="5"/>
       <c r="J85" s="29"/>
     </row>
     <row r="86" spans="1:11" ht="12.75" customHeight="1">
       <c r="A86" s="33" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="B86" s="15" t="s">
         <v>290</v>
       </c>
       <c r="C86" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D86" s="33" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E86" s="11">
         <v>92</v>
@@ -4767,16 +4757,16 @@
     </row>
     <row r="87" spans="1:11" s="17" customFormat="1" ht="12.75" customHeight="1">
       <c r="A87" s="33" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="B87" s="15" t="s">
         <v>67</v>
       </c>
       <c r="C87" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D87" s="33" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="E87" s="11">
         <v>85</v>
@@ -4785,26 +4775,26 @@
         <v>6</v>
       </c>
       <c r="G87" s="15" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="H87" s="15" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="I87" s="11"/>
       <c r="J87" s="11"/>
     </row>
     <row r="88" spans="1:11" s="17" customFormat="1" ht="12.75" customHeight="1">
       <c r="A88" s="33" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="B88" s="15" t="s">
         <v>249</v>
       </c>
       <c r="C88" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D88" s="33" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E88" s="11">
         <v>85</v>
@@ -4813,26 +4803,26 @@
         <v>8</v>
       </c>
       <c r="G88" s="15" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="H88" s="15" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="I88" s="11"/>
       <c r="J88" s="11"/>
     </row>
     <row r="89" spans="1:11" s="17" customFormat="1" ht="12.75" customHeight="1">
       <c r="A89" s="33" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B89" s="4" t="s">
         <v>215</v>
       </c>
       <c r="C89" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D89" s="33" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E89" s="6">
         <v>90</v>
@@ -4841,7 +4831,7 @@
         <v>9</v>
       </c>
       <c r="G89" s="4" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="H89" s="4"/>
       <c r="I89" s="6"/>
@@ -4850,16 +4840,16 @@
     </row>
     <row r="90" spans="1:11" s="17" customFormat="1" ht="12.75" customHeight="1">
       <c r="A90" s="33" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="B90" s="4" t="s">
         <v>47</v>
       </c>
       <c r="C90" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D90" s="33" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E90" s="6">
         <v>95</v>
@@ -4868,10 +4858,10 @@
         <v>10</v>
       </c>
       <c r="G90" s="15" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="H90" s="4" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="I90" s="6"/>
       <c r="J90" s="6"/>
@@ -4879,16 +4869,16 @@
     </row>
     <row r="91" spans="1:11" s="1" customFormat="1" ht="12.75" customHeight="1">
       <c r="A91" s="33" t="s">
+        <v>436</v>
+      </c>
+      <c r="B91" s="4" t="s">
         <v>437</v>
       </c>
-      <c r="B91" s="4" t="s">
-        <v>438</v>
-      </c>
       <c r="C91" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D91" s="33" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="E91" s="6">
         <v>90</v>
@@ -4897,36 +4887,36 @@
         <v>7</v>
       </c>
       <c r="G91" s="4" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="H91" s="4" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="I91" s="4"/>
       <c r="J91" s="29"/>
     </row>
     <row r="92" spans="1:11" s="32" customFormat="1" ht="12.75" customHeight="1">
       <c r="A92" s="40" t="s">
+        <v>442</v>
+      </c>
+      <c r="B92" s="15" t="s">
         <v>443</v>
       </c>
-      <c r="B92" s="15" t="s">
-        <v>444</v>
-      </c>
       <c r="C92" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D92" s="33" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="E92" s="11">
         <v>87</v>
       </c>
       <c r="F92" s="10"/>
       <c r="G92" s="15" t="s">
+        <v>558</v>
+      </c>
+      <c r="H92" s="15" t="s">
         <v>559</v>
-      </c>
-      <c r="H92" s="15" t="s">
-        <v>560</v>
       </c>
       <c r="I92" s="31"/>
       <c r="J92" s="31"/>
@@ -4936,13 +4926,13 @@
         <v>325</v>
       </c>
       <c r="B93" s="15" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="C93" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D93" s="33" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="E93" s="11">
         <v>85</v>
@@ -4951,26 +4941,26 @@
         <v>11</v>
       </c>
       <c r="G93" s="15" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="H93" s="15" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="I93" s="11"/>
       <c r="J93" s="11"/>
     </row>
     <row r="94" spans="1:11" s="17" customFormat="1" ht="12.75" customHeight="1">
       <c r="A94" s="33" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B94" s="15" t="s">
         <v>57</v>
       </c>
       <c r="C94" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D94" s="33" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E94" s="11">
         <v>85</v>
@@ -4989,16 +4979,16 @@
     </row>
     <row r="95" spans="1:11" s="17" customFormat="1" ht="12.75" customHeight="1">
       <c r="A95" s="33" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B95" s="15" t="s">
         <v>56</v>
       </c>
       <c r="C95" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D95" s="33" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E95" s="6">
         <v>85</v>
@@ -5024,10 +5014,10 @@
         <v>69</v>
       </c>
       <c r="C96" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D96" s="33" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E96" s="11">
         <v>85</v>
@@ -5046,42 +5036,42 @@
     </row>
     <row r="97" spans="1:11" s="17" customFormat="1" ht="12.75" customHeight="1">
       <c r="A97" s="33" t="s">
+        <v>553</v>
+      </c>
+      <c r="B97" s="15" t="s">
         <v>554</v>
       </c>
-      <c r="B97" s="15" t="s">
-        <v>555</v>
-      </c>
       <c r="C97" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D97" s="33" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E97" s="11">
         <v>85</v>
       </c>
       <c r="F97" s="11"/>
       <c r="G97" s="15" t="s">
+        <v>555</v>
+      </c>
+      <c r="H97" s="15" t="s">
         <v>556</v>
-      </c>
-      <c r="H97" s="15" t="s">
-        <v>557</v>
       </c>
       <c r="I97" s="11"/>
       <c r="J97" s="11"/>
     </row>
     <row r="98" spans="1:11" s="17" customFormat="1" ht="12.75" customHeight="1">
       <c r="A98" s="33" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="B98" s="15" t="s">
         <v>279</v>
       </c>
       <c r="C98" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D98" s="33" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E98" s="11">
         <v>85</v>
@@ -5098,16 +5088,16 @@
     </row>
     <row r="99" spans="1:11" s="17" customFormat="1" ht="12.75" customHeight="1">
       <c r="A99" s="33" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="B99" s="4" t="s">
         <v>51</v>
       </c>
       <c r="C99" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D99" s="33" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E99" s="6">
         <v>85</v>
@@ -5116,7 +5106,7 @@
         <v>16</v>
       </c>
       <c r="G99" s="4" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="H99" s="4" t="s">
         <v>273</v>
@@ -5133,10 +5123,10 @@
         <v>313</v>
       </c>
       <c r="C100" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D100" s="33" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E100" s="6">
         <v>85</v>
@@ -5145,10 +5135,10 @@
         <v>17</v>
       </c>
       <c r="G100" s="15" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="H100" s="15" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="J100" s="11"/>
     </row>
@@ -5160,10 +5150,10 @@
         <v>248</v>
       </c>
       <c r="C101" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D101" s="33" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E101" s="11">
         <v>85</v>
@@ -5183,16 +5173,16 @@
     </row>
     <row r="102" spans="1:11" s="15" customFormat="1" ht="12.75" customHeight="1">
       <c r="A102" s="33" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="B102" s="15" t="s">
         <v>259</v>
       </c>
       <c r="C102" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D102" s="33" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E102" s="11">
         <v>83</v>
@@ -5212,16 +5202,16 @@
     </row>
     <row r="103" spans="1:11" ht="12.75" customHeight="1">
       <c r="A103" s="40" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B103" s="15" t="s">
         <v>61</v>
       </c>
       <c r="C103" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D103" s="33" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E103" s="11">
         <v>80</v>
@@ -5245,10 +5235,10 @@
         <v>50</v>
       </c>
       <c r="C104" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D104" s="33" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E104" s="11">
         <v>82</v>
@@ -5274,10 +5264,10 @@
         <v>320</v>
       </c>
       <c r="C105" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D105" s="33" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E105" s="6">
         <v>85</v>
@@ -5286,10 +5276,10 @@
         <v>22</v>
       </c>
       <c r="G105" s="4" t="s">
+        <v>365</v>
+      </c>
+      <c r="H105" s="11" t="s">
         <v>366</v>
-      </c>
-      <c r="H105" s="11" t="s">
-        <v>367</v>
       </c>
       <c r="I105" s="2"/>
       <c r="J105" s="6"/>
@@ -5303,7 +5293,7 @@
         <v>203</v>
       </c>
       <c r="C106" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D106" s="37" t="s">
         <v>101</v>
@@ -5315,7 +5305,7 @@
         <v>23</v>
       </c>
       <c r="G106" s="4" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="H106" s="4"/>
       <c r="I106" s="6"/>
@@ -5328,10 +5318,10 @@
         <v>14</v>
       </c>
       <c r="C107" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D107" s="33" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E107" s="6">
         <v>80</v>
@@ -5347,16 +5337,16 @@
     </row>
     <row r="108" spans="1:11" s="17" customFormat="1" ht="12.75" customHeight="1">
       <c r="A108" s="33" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B108" s="15" t="s">
         <v>63</v>
       </c>
       <c r="C108" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D108" s="33" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E108" s="11">
         <v>85</v>
@@ -5375,16 +5365,16 @@
     </row>
     <row r="109" spans="1:11" s="17" customFormat="1" ht="12.75" customHeight="1">
       <c r="A109" s="33" t="s">
+        <v>373</v>
+      </c>
+      <c r="B109" s="4" t="s">
         <v>374</v>
       </c>
-      <c r="B109" s="4" t="s">
-        <v>375</v>
-      </c>
       <c r="C109" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D109" s="33" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E109" s="6">
         <v>78</v>
@@ -5393,10 +5383,10 @@
         <v>26</v>
       </c>
       <c r="G109" s="4" t="s">
+        <v>375</v>
+      </c>
+      <c r="H109" s="4" t="s">
         <v>376</v>
-      </c>
-      <c r="H109" s="4" t="s">
-        <v>377</v>
       </c>
       <c r="I109" s="6"/>
       <c r="J109" s="6"/>
@@ -5410,10 +5400,10 @@
         <v>202</v>
       </c>
       <c r="C110" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D110" s="33" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E110" s="6">
         <v>80</v>
@@ -5429,16 +5419,16 @@
     </row>
     <row r="111" spans="1:11" ht="12.75" customHeight="1">
       <c r="A111" s="33" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="B111" s="15" t="s">
         <v>58</v>
       </c>
       <c r="C111" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D111" s="33" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E111" s="11">
         <v>80</v>
@@ -5447,7 +5437,7 @@
         <v>28</v>
       </c>
       <c r="G111" s="15" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="H111" s="15" t="s">
         <v>324</v>
@@ -5464,10 +5454,10 @@
         <v>66</v>
       </c>
       <c r="C112" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D112" s="33" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E112" s="11">
         <v>77</v>
@@ -5492,10 +5482,10 @@
         <v>70</v>
       </c>
       <c r="C113" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D113" s="33" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E113" s="11">
         <v>75</v>
@@ -5514,42 +5504,42 @@
     </row>
     <row r="114" spans="1:11" s="17" customFormat="1" ht="12.75" customHeight="1">
       <c r="A114" s="15" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B114" s="15" t="s">
         <v>76</v>
       </c>
       <c r="C114" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D114" s="33" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="E114" s="11">
         <v>85</v>
       </c>
       <c r="F114" s="11"/>
       <c r="G114" s="15" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="H114" s="15" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="I114" s="11"/>
       <c r="J114" s="11"/>
     </row>
     <row r="115" spans="1:11" s="17" customFormat="1" ht="12.75" customHeight="1">
       <c r="A115" s="33" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="B115" s="15" t="s">
         <v>301</v>
       </c>
       <c r="C115" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D115" s="33" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E115" s="11">
         <v>85</v>
@@ -5570,10 +5560,10 @@
         <v>59</v>
       </c>
       <c r="C116" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D116" s="33" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E116" s="6">
         <v>85</v>
@@ -5589,23 +5579,23 @@
     </row>
     <row r="117" spans="1:11" ht="12.75" customHeight="1">
       <c r="A117" s="33" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="B117" s="15" t="s">
         <v>322</v>
       </c>
       <c r="C117" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D117" s="33" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E117" s="6">
         <v>85</v>
       </c>
       <c r="F117" s="15"/>
       <c r="G117" s="15" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="H117" s="15" t="s">
         <v>323</v>
@@ -5622,10 +5612,10 @@
         <v>228</v>
       </c>
       <c r="C118" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D118" s="33" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E118" s="6">
         <v>75</v>
@@ -5638,16 +5628,16 @@
     </row>
     <row r="119" spans="1:11" s="4" customFormat="1" ht="12.75" customHeight="1">
       <c r="A119" s="33" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="B119" s="4" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C119" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D119" s="33" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E119" s="6">
         <v>75</v>
@@ -5662,16 +5652,16 @@
     </row>
     <row r="120" spans="1:11" s="17" customFormat="1" ht="12.75" customHeight="1">
       <c r="A120" s="37" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="B120" s="4" t="s">
         <v>45</v>
       </c>
       <c r="C120" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D120" s="33" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E120" s="6">
         <v>75</v>
@@ -5695,10 +5685,10 @@
         <v>11</v>
       </c>
       <c r="C121" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D121" s="33" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E121" s="6">
         <v>75</v>
@@ -5717,10 +5707,10 @@
         <v>208</v>
       </c>
       <c r="C122" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D122" s="33" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E122" s="6">
         <v>75</v>
@@ -5733,26 +5723,26 @@
     </row>
     <row r="123" spans="1:11" s="17" customFormat="1" ht="12.75" customHeight="1">
       <c r="A123" s="33" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B123" s="15" t="s">
         <v>68</v>
       </c>
       <c r="C123" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D123" s="33" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E123" s="11">
         <v>75</v>
       </c>
       <c r="F123" s="11"/>
       <c r="G123" s="15" t="s">
+        <v>338</v>
+      </c>
+      <c r="H123" s="15" t="s">
         <v>339</v>
-      </c>
-      <c r="H123" s="15" t="s">
-        <v>340</v>
       </c>
       <c r="I123" s="11"/>
       <c r="J123" s="11"/>
@@ -5765,10 +5755,10 @@
         <v>288</v>
       </c>
       <c r="C124" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D124" s="33" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E124" s="6">
         <v>75</v>
@@ -5783,22 +5773,22 @@
     </row>
     <row r="125" spans="1:11" ht="12.75" customHeight="1">
       <c r="A125" s="33" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B125" s="4" t="s">
         <v>210</v>
       </c>
       <c r="C125" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D125" s="33" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E125" s="6">
         <v>75</v>
       </c>
       <c r="G125" s="4" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="H125" s="4"/>
       <c r="I125" s="6"/>
@@ -5811,32 +5801,32 @@
         <v>204</v>
       </c>
       <c r="C126" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D126" s="33" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E126" s="6">
         <v>70</v>
       </c>
       <c r="G126" s="4" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="H126" s="4"/>
       <c r="I126" s="6"/>
     </row>
     <row r="127" spans="1:11" ht="12.75" customHeight="1">
       <c r="A127" s="33" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B127" s="15" t="s">
         <v>64</v>
       </c>
       <c r="C127" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D127" s="33" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E127" s="11">
         <v>70</v>
@@ -5858,10 +5848,10 @@
         <v>207</v>
       </c>
       <c r="C128" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D128" s="33" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E128" s="6">
         <v>70</v>
@@ -5874,16 +5864,16 @@
     </row>
     <row r="129" spans="1:11" s="17" customFormat="1" ht="12.75" customHeight="1">
       <c r="A129" s="33" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B129" s="4" t="s">
         <v>39</v>
       </c>
       <c r="C129" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D129" s="33" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E129" s="6">
         <v>70</v>
@@ -5899,16 +5889,16 @@
     </row>
     <row r="130" spans="1:11" ht="12.75" customHeight="1">
       <c r="A130" s="33" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="B130" s="4" t="s">
         <v>211</v>
       </c>
       <c r="C130" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D130" s="33" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E130" s="6">
         <v>70</v>
@@ -5927,10 +5917,10 @@
         <v>212</v>
       </c>
       <c r="C131" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D131" s="33" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E131" s="6">
         <v>70</v>
@@ -5946,26 +5936,26 @@
     </row>
     <row r="132" spans="1:11" s="17" customFormat="1" ht="12.75" customHeight="1">
       <c r="A132" s="33" t="s">
+        <v>418</v>
+      </c>
+      <c r="B132" s="4" t="s">
         <v>419</v>
       </c>
-      <c r="B132" s="4" t="s">
-        <v>420</v>
-      </c>
       <c r="C132" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D132" s="33" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E132" s="6">
         <v>70</v>
       </c>
       <c r="F132" s="6"/>
       <c r="G132" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="H132" s="4" t="s">
         <v>421</v>
-      </c>
-      <c r="H132" s="4" t="s">
-        <v>422</v>
       </c>
       <c r="I132" s="6"/>
       <c r="J132" s="6"/>
@@ -5973,16 +5963,16 @@
     </row>
     <row r="133" spans="1:11" ht="12.75" customHeight="1">
       <c r="A133" s="33" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="B133" s="4" t="s">
         <v>46</v>
       </c>
       <c r="C133" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D133" s="33" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E133" s="6">
         <v>65</v>
@@ -6001,10 +5991,10 @@
         <v>205</v>
       </c>
       <c r="C134" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D134" s="33" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E134" s="6">
         <v>60</v>
@@ -6017,16 +6007,16 @@
     </row>
     <row r="135" spans="1:11" ht="12.75" customHeight="1">
       <c r="A135" s="35" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="B135" s="12" t="s">
         <v>49</v>
       </c>
       <c r="C135" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D135" s="35" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E135" s="10"/>
       <c r="F135" s="10"/>
@@ -6038,16 +6028,16 @@
     </row>
     <row r="136" spans="1:11" s="23" customFormat="1" ht="12.75" customHeight="1">
       <c r="A136" s="35" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="B136" s="12" t="s">
         <v>55</v>
       </c>
       <c r="C136" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D136" s="35" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E136" s="10"/>
       <c r="F136" s="10"/>
@@ -6066,10 +6056,10 @@
         <v>306</v>
       </c>
       <c r="C137" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D137" s="35" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E137" s="10"/>
       <c r="F137" s="10"/>
@@ -6081,16 +6071,16 @@
     </row>
     <row r="138" spans="1:11" s="23" customFormat="1" ht="12.75" customHeight="1">
       <c r="A138" s="35" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="B138" s="12" t="s">
         <v>75</v>
       </c>
       <c r="C138" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D138" s="35" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E138" s="10"/>
       <c r="F138" s="10"/>
@@ -6103,16 +6093,16 @@
     </row>
     <row r="139" spans="1:11" ht="12.75" customHeight="1">
       <c r="A139" s="35" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="B139" s="12" t="s">
         <v>62</v>
       </c>
       <c r="C139" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D139" s="35" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E139" s="10"/>
       <c r="F139" s="10"/>
@@ -6124,16 +6114,16 @@
     </row>
     <row r="140" spans="1:11" ht="12.75" customHeight="1">
       <c r="A140" s="35" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B140" s="12" t="s">
         <v>77</v>
       </c>
       <c r="C140" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D140" s="35" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E140" s="10"/>
       <c r="F140" s="10"/>
@@ -6151,10 +6141,10 @@
         <v>304</v>
       </c>
       <c r="C141" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D141" s="35" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E141" s="10"/>
       <c r="F141" s="10"/>
@@ -6167,16 +6157,16 @@
     </row>
     <row r="142" spans="1:11" ht="12.75" customHeight="1">
       <c r="A142" s="35" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="B142" s="12" t="s">
         <v>48</v>
       </c>
       <c r="C142" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D142" s="35" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E142" s="10"/>
       <c r="F142" s="10"/>
@@ -6186,16 +6176,16 @@
     </row>
     <row r="143" spans="1:11" ht="12.75" customHeight="1">
       <c r="A143" s="35" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="B143" s="12" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="C143" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D143" s="35" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="E143" s="10"/>
       <c r="F143" s="10"/>
@@ -6205,13 +6195,13 @@
     </row>
     <row r="144" spans="1:11" ht="12.75" customHeight="1">
       <c r="A144" s="35" t="s">
+        <v>568</v>
+      </c>
+      <c r="B144" s="12" t="s">
         <v>569</v>
       </c>
-      <c r="B144" s="12" t="s">
-        <v>570</v>
-      </c>
       <c r="C144" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D144" s="35"/>
       <c r="E144" s="10"/>
@@ -6222,16 +6212,16 @@
     </row>
     <row r="145" spans="1:9" ht="12.75" customHeight="1">
       <c r="A145" s="35" t="s">
+        <v>389</v>
+      </c>
+      <c r="B145" s="12" t="s">
         <v>390</v>
       </c>
-      <c r="B145" s="12" t="s">
-        <v>391</v>
-      </c>
       <c r="C145" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D145" s="35" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E145" s="10"/>
       <c r="F145" s="10"/>
@@ -6241,16 +6231,16 @@
     </row>
     <row r="146" spans="1:9" ht="12.75" customHeight="1">
       <c r="A146" s="35" t="s">
+        <v>359</v>
+      </c>
+      <c r="B146" s="12" t="s">
         <v>360</v>
       </c>
-      <c r="B146" s="12" t="s">
-        <v>361</v>
-      </c>
       <c r="C146" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D146" s="35" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E146" s="10"/>
       <c r="F146" s="10"/>
@@ -6260,16 +6250,16 @@
     </row>
     <row r="147" spans="1:9" ht="12.75" customHeight="1">
       <c r="A147" s="35" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="B147" s="12" t="s">
         <v>247</v>
       </c>
       <c r="C147" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D147" s="35" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E147" s="10"/>
       <c r="F147" s="10"/>
@@ -6285,10 +6275,10 @@
         <v>52</v>
       </c>
       <c r="C148" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D148" s="35" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="E148" s="10"/>
       <c r="F148" s="10"/>
@@ -6298,16 +6288,16 @@
     </row>
     <row r="149" spans="1:9" ht="12.75" customHeight="1">
       <c r="A149" s="35" t="s">
+        <v>391</v>
+      </c>
+      <c r="B149" s="12" t="s">
         <v>392</v>
       </c>
-      <c r="B149" s="12" t="s">
-        <v>393</v>
-      </c>
       <c r="C149" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D149" s="35" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E149" s="10"/>
       <c r="F149" s="10"/>
@@ -6317,16 +6307,16 @@
     </row>
     <row r="150" spans="1:9" ht="12.75" customHeight="1">
       <c r="A150" s="35" t="s">
+        <v>393</v>
+      </c>
+      <c r="B150" s="12" t="s">
         <v>394</v>
       </c>
-      <c r="B150" s="12" t="s">
-        <v>395</v>
-      </c>
       <c r="C150" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D150" s="35" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="E150" s="10"/>
       <c r="F150" s="10"/>
@@ -6336,16 +6326,16 @@
     </row>
     <row r="151" spans="1:9" ht="12.75" customHeight="1">
       <c r="A151" s="35" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B151" s="12" t="s">
         <v>54</v>
       </c>
       <c r="C151" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D151" s="35" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E151" s="10"/>
       <c r="F151" s="10"/>
@@ -6355,13 +6345,13 @@
     </row>
     <row r="152" spans="1:9" ht="12.75" customHeight="1">
       <c r="A152" s="35" t="s">
+        <v>570</v>
+      </c>
+      <c r="B152" s="12" t="s">
         <v>571</v>
       </c>
-      <c r="B152" s="12" t="s">
-        <v>572</v>
-      </c>
       <c r="C152" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D152" s="35"/>
       <c r="E152" s="10"/>
@@ -6372,13 +6362,13 @@
     </row>
     <row r="153" spans="1:9" ht="12.75" customHeight="1">
       <c r="A153" s="35" t="s">
+        <v>572</v>
+      </c>
+      <c r="B153" s="12" t="s">
         <v>573</v>
       </c>
-      <c r="B153" s="12" t="s">
-        <v>574</v>
-      </c>
       <c r="C153" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D153" s="35"/>
       <c r="E153" s="10"/>
@@ -6389,13 +6379,13 @@
     </row>
     <row r="154" spans="1:9" ht="12.75" customHeight="1">
       <c r="A154" s="35" t="s">
+        <v>574</v>
+      </c>
+      <c r="B154" s="12" t="s">
         <v>575</v>
       </c>
-      <c r="B154" s="12" t="s">
-        <v>576</v>
-      </c>
       <c r="C154" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D154" s="35"/>
       <c r="E154" s="10"/>
@@ -6406,16 +6396,16 @@
     </row>
     <row r="155" spans="1:9" ht="12.75" customHeight="1">
       <c r="A155" s="35" t="s">
+        <v>396</v>
+      </c>
+      <c r="B155" s="12" t="s">
         <v>397</v>
       </c>
-      <c r="B155" s="12" t="s">
-        <v>398</v>
-      </c>
       <c r="C155" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D155" s="35" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E155" s="10"/>
       <c r="F155" s="10"/>
@@ -6425,13 +6415,13 @@
     </row>
     <row r="156" spans="1:9" ht="12.75" customHeight="1">
       <c r="A156" s="35" t="s">
+        <v>576</v>
+      </c>
+      <c r="B156" s="12" t="s">
         <v>577</v>
       </c>
-      <c r="B156" s="12" t="s">
-        <v>578</v>
-      </c>
       <c r="C156" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D156" s="35"/>
       <c r="E156" s="10"/>
@@ -6442,16 +6432,16 @@
     </row>
     <row r="157" spans="1:9" ht="12.75" customHeight="1">
       <c r="A157" s="35" t="s">
+        <v>398</v>
+      </c>
+      <c r="B157" s="12" t="s">
         <v>399</v>
       </c>
-      <c r="B157" s="12" t="s">
-        <v>400</v>
-      </c>
       <c r="C157" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D157" s="35" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="E157" s="10"/>
       <c r="F157" s="10"/>
@@ -6461,13 +6451,13 @@
     </row>
     <row r="158" spans="1:9" ht="12.75" customHeight="1">
       <c r="A158" s="35" t="s">
+        <v>578</v>
+      </c>
+      <c r="B158" s="12" t="s">
         <v>579</v>
       </c>
-      <c r="B158" s="12" t="s">
-        <v>580</v>
-      </c>
       <c r="C158" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D158" s="35"/>
       <c r="E158" s="10"/>
@@ -6478,16 +6468,16 @@
     </row>
     <row r="159" spans="1:9" ht="12.75" customHeight="1">
       <c r="A159" s="35" t="s">
+        <v>400</v>
+      </c>
+      <c r="B159" s="12" t="s">
         <v>401</v>
       </c>
-      <c r="B159" s="12" t="s">
-        <v>402</v>
-      </c>
       <c r="C159" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D159" s="35" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E159" s="10"/>
       <c r="F159" s="10"/>
@@ -6497,16 +6487,16 @@
     </row>
     <row r="160" spans="1:9" ht="12.75" customHeight="1">
       <c r="A160" s="35" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B160" s="12" t="s">
         <v>60</v>
       </c>
       <c r="C160" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D160" s="35" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E160" s="10"/>
       <c r="F160" s="10"/>
@@ -6516,16 +6506,16 @@
     </row>
     <row r="161" spans="1:10" ht="12.75" customHeight="1">
       <c r="A161" s="35" t="s">
+        <v>402</v>
+      </c>
+      <c r="B161" s="12" t="s">
         <v>403</v>
       </c>
-      <c r="B161" s="12" t="s">
-        <v>404</v>
-      </c>
       <c r="C161" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D161" s="35" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E161" s="10"/>
       <c r="F161" s="10"/>
@@ -6535,16 +6525,16 @@
     </row>
     <row r="162" spans="1:10" ht="12.75" customHeight="1">
       <c r="A162" s="35" t="s">
+        <v>508</v>
+      </c>
+      <c r="B162" s="12" t="s">
         <v>509</v>
       </c>
-      <c r="B162" s="12" t="s">
-        <v>510</v>
-      </c>
       <c r="C162" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D162" s="35" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E162" s="10"/>
       <c r="F162" s="10"/>
@@ -6554,16 +6544,16 @@
     </row>
     <row r="163" spans="1:10" ht="12.75" customHeight="1">
       <c r="A163" s="35" t="s">
+        <v>369</v>
+      </c>
+      <c r="B163" s="12" t="s">
         <v>370</v>
       </c>
-      <c r="B163" s="12" t="s">
-        <v>371</v>
-      </c>
       <c r="C163" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D163" s="35" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="E163" s="10"/>
       <c r="F163" s="10"/>
@@ -6579,10 +6569,10 @@
         <v>65</v>
       </c>
       <c r="C164" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D164" s="35" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="E164" s="10"/>
       <c r="F164" s="10"/>
@@ -6593,16 +6583,16 @@
     </row>
     <row r="165" spans="1:10" s="32" customFormat="1" ht="12.75" customHeight="1">
       <c r="A165" s="35" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B165" s="12" t="s">
         <v>250</v>
       </c>
       <c r="C165" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D165" s="35" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="E165" s="30"/>
       <c r="F165" s="30"/>
@@ -6613,16 +6603,16 @@
     </row>
     <row r="166" spans="1:10" ht="12.75" customHeight="1">
       <c r="A166" s="35" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="B166" s="12" t="s">
         <v>51</v>
       </c>
       <c r="C166" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D166" s="35" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E166" s="10"/>
       <c r="F166" s="10"/>
@@ -6632,16 +6622,16 @@
     </row>
     <row r="167" spans="1:10" ht="12.75" customHeight="1">
       <c r="A167" s="35" t="s">
+        <v>566</v>
+      </c>
+      <c r="B167" s="12" t="s">
         <v>567</v>
       </c>
-      <c r="B167" s="12" t="s">
-        <v>568</v>
-      </c>
       <c r="C167" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D167" s="35" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E167" s="10"/>
       <c r="F167" s="10"/>
@@ -6651,16 +6641,16 @@
     </row>
     <row r="168" spans="1:10" ht="12.75" customHeight="1">
       <c r="A168" s="35" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B168" s="12" t="s">
         <v>256</v>
       </c>
       <c r="C168" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D168" s="35" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E168" s="10"/>
       <c r="F168" s="10"/>
@@ -6670,16 +6660,16 @@
     </row>
     <row r="169" spans="1:10" ht="12.75" customHeight="1">
       <c r="A169" s="12" t="s">
+        <v>439</v>
+      </c>
+      <c r="B169" s="12" t="s">
         <v>440</v>
       </c>
-      <c r="B169" s="12" t="s">
-        <v>441</v>
-      </c>
       <c r="C169" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D169" s="35" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="E169" s="10"/>
       <c r="F169" s="10"/>
@@ -6689,13 +6679,13 @@
     </row>
     <row r="170" spans="1:10" ht="12.75" customHeight="1">
       <c r="A170" s="12" t="s">
+        <v>580</v>
+      </c>
+      <c r="B170" s="12" t="s">
         <v>581</v>
       </c>
-      <c r="B170" s="12" t="s">
-        <v>582</v>
-      </c>
       <c r="C170" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D170" s="35"/>
       <c r="E170" s="10"/>
@@ -6706,16 +6696,16 @@
     </row>
     <row r="171" spans="1:10" ht="12.75" customHeight="1">
       <c r="A171" s="35" t="s">
+        <v>516</v>
+      </c>
+      <c r="B171" s="12" t="s">
         <v>517</v>
       </c>
-      <c r="B171" s="12" t="s">
-        <v>518</v>
-      </c>
       <c r="C171" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D171" s="35" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E171" s="10"/>
       <c r="F171" s="10"/>
@@ -6725,16 +6715,16 @@
     </row>
     <row r="172" spans="1:10" s="23" customFormat="1" ht="12.75" customHeight="1">
       <c r="A172" s="35" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="B172" s="12" t="s">
         <v>299</v>
       </c>
       <c r="C172" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D172" s="35" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E172" s="10"/>
       <c r="F172" s="10"/>
@@ -6745,13 +6735,13 @@
     </row>
     <row r="173" spans="1:10" s="23" customFormat="1" ht="12.75" customHeight="1">
       <c r="A173" s="35" t="s">
+        <v>582</v>
+      </c>
+      <c r="B173" s="12" t="s">
         <v>583</v>
       </c>
-      <c r="B173" s="12" t="s">
-        <v>584</v>
-      </c>
       <c r="C173" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D173" s="35"/>
       <c r="E173" s="10"/>
@@ -6763,9 +6753,6 @@
     </row>
     <row r="174" spans="1:10" ht="12.75" customHeight="1">
       <c r="A174" s="1"/>
-      <c r="C174" s="4" t="s">
-        <v>608</v>
-      </c>
       <c r="D174" s="12"/>
       <c r="G174" s="4"/>
       <c r="H174" s="6"/>
@@ -6776,7 +6763,7 @@
         <v>71</v>
       </c>
       <c r="C175" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D175" s="12"/>
       <c r="G175" s="4"/>
@@ -6789,7 +6776,7 @@
       </c>
       <c r="B176" s="13"/>
       <c r="C176" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D176" s="13"/>
       <c r="E176" s="20">
@@ -6807,11 +6794,11 @@
     </row>
     <row r="177" spans="1:10" s="19" customFormat="1" ht="12.75" customHeight="1">
       <c r="A177" s="19" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="B177" s="13"/>
       <c r="C177" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D177" s="13"/>
       <c r="E177" s="20">
@@ -6828,7 +6815,7 @@
         <v>120</v>
       </c>
       <c r="C178" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="E178" s="6">
         <v>85</v>
@@ -6847,7 +6834,7 @@
         <v>121</v>
       </c>
       <c r="C179" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="E179" s="6">
         <v>85</v>
@@ -6863,16 +6850,16 @@
     </row>
     <row r="180" spans="1:10" ht="12.75" customHeight="1">
       <c r="A180" s="4" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="C180" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="E180" s="6">
         <v>85</v>
       </c>
       <c r="G180" s="4" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="H180" s="6"/>
       <c r="I180" s="6"/>
@@ -6882,7 +6869,7 @@
         <v>325</v>
       </c>
       <c r="C181" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="E181" s="6">
         <v>85</v>
@@ -6898,7 +6885,7 @@
         <v>107</v>
       </c>
       <c r="C182" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="E182" s="6">
         <v>85</v>
@@ -6914,7 +6901,7 @@
         <v>125</v>
       </c>
       <c r="C183" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="E183" s="6">
         <v>80</v>
@@ -6930,10 +6917,10 @@
     </row>
     <row r="184" spans="1:10" ht="12.75" customHeight="1">
       <c r="A184" s="4" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C184" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="E184" s="6">
         <v>80</v>
@@ -6944,10 +6931,10 @@
     </row>
     <row r="185" spans="1:10" ht="12.75" customHeight="1">
       <c r="A185" s="4" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C185" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="E185" s="6">
         <v>80</v>
@@ -6958,32 +6945,32 @@
     </row>
     <row r="186" spans="1:10" ht="12.75" customHeight="1">
       <c r="A186" s="4" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C186" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="E186" s="6">
         <v>80</v>
       </c>
       <c r="G186" s="4" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="H186" s="6"/>
       <c r="I186" s="6"/>
     </row>
     <row r="187" spans="1:10" ht="12.75" customHeight="1">
       <c r="A187" s="4" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="C187" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="E187" s="6">
         <v>80</v>
       </c>
       <c r="G187" s="4" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="H187" s="6"/>
       <c r="I187" s="6"/>
@@ -6993,7 +6980,7 @@
         <v>264</v>
       </c>
       <c r="C188" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="E188" s="6">
         <v>80</v>
@@ -7009,7 +6996,7 @@
         <v>117</v>
       </c>
       <c r="C189" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="E189" s="6">
         <v>75</v>
@@ -7023,7 +7010,7 @@
         <v>119</v>
       </c>
       <c r="C190" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="E190" s="6">
         <v>75</v>
@@ -7042,13 +7029,13 @@
         <v>129</v>
       </c>
       <c r="C191" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="E191" s="6">
         <v>75</v>
       </c>
       <c r="G191" s="4" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="H191" s="6"/>
       <c r="I191" s="6"/>
@@ -7058,7 +7045,7 @@
         <v>102</v>
       </c>
       <c r="C192" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="E192" s="6">
         <v>75</v>
@@ -7072,7 +7059,7 @@
         <v>261</v>
       </c>
       <c r="C193" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="E193" s="6">
         <v>75</v>
@@ -7088,7 +7075,7 @@
         <v>128</v>
       </c>
       <c r="C194" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="E194" s="6">
         <v>75</v>
@@ -7102,7 +7089,7 @@
         <v>130</v>
       </c>
       <c r="C195" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="E195" s="6">
         <v>75</v>
@@ -7119,7 +7106,7 @@
         <v>106</v>
       </c>
       <c r="C196" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="E196" s="6">
         <v>75</v>
@@ -7138,7 +7125,7 @@
         <v>137</v>
       </c>
       <c r="C197" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="E197" s="6">
         <v>75</v>
@@ -7152,16 +7139,16 @@
     </row>
     <row r="198" spans="1:9" ht="12.75" customHeight="1">
       <c r="A198" s="4" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="C198" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="E198" s="6">
         <v>70</v>
       </c>
       <c r="G198" s="4" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="H198" s="6"/>
       <c r="I198" s="6"/>
@@ -7171,7 +7158,7 @@
         <v>118</v>
       </c>
       <c r="C199" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="E199" s="6">
         <v>70</v>
@@ -7185,7 +7172,7 @@
         <v>122</v>
       </c>
       <c r="C200" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="E200" s="6">
         <v>70</v>
@@ -7199,7 +7186,7 @@
         <v>123</v>
       </c>
       <c r="C201" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="E201" s="6">
         <v>70</v>
@@ -7215,7 +7202,7 @@
         <v>263</v>
       </c>
       <c r="C202" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="E202" s="6">
         <v>70</v>
@@ -7229,7 +7216,7 @@
         <v>126</v>
       </c>
       <c r="C203" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="E203" s="6">
         <v>70</v>
@@ -7243,29 +7230,29 @@
         <v>127</v>
       </c>
       <c r="C204" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="E204" s="6">
         <v>70</v>
       </c>
       <c r="G204" s="4" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="H204" s="6"/>
       <c r="I204" s="6"/>
     </row>
     <row r="205" spans="1:9" ht="12.75" customHeight="1">
       <c r="A205" s="4" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C205" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="E205" s="6">
         <v>70</v>
       </c>
       <c r="G205" s="4" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="H205" s="6"/>
       <c r="I205" s="6"/>
@@ -7275,7 +7262,7 @@
         <v>129</v>
       </c>
       <c r="C206" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="E206" s="6">
         <v>70</v>
@@ -7289,7 +7276,7 @@
         <v>131</v>
       </c>
       <c r="C207" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="E207" s="6">
         <v>70</v>
@@ -7303,13 +7290,13 @@
         <v>133</v>
       </c>
       <c r="C208" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="E208" s="6">
         <v>70</v>
       </c>
       <c r="G208" s="4" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="H208" s="6"/>
       <c r="I208" s="6"/>
@@ -7319,7 +7306,7 @@
         <v>135</v>
       </c>
       <c r="C209" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="E209" s="6">
         <v>70</v>
@@ -7335,7 +7322,7 @@
         <v>132</v>
       </c>
       <c r="C210" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="E210" s="6">
         <v>65</v>
@@ -7351,7 +7338,7 @@
         <v>136</v>
       </c>
       <c r="C211" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="E211" s="6">
         <v>65</v>
@@ -7365,7 +7352,7 @@
         <v>138</v>
       </c>
       <c r="C212" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="E212" s="6">
         <v>65</v>
@@ -7379,7 +7366,7 @@
         <v>116</v>
       </c>
       <c r="C213" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="E213" s="6">
         <v>60</v>
@@ -7393,7 +7380,7 @@
         <v>103</v>
       </c>
       <c r="C214" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="E214" s="6">
         <v>60</v>
@@ -7407,7 +7394,7 @@
         <v>134</v>
       </c>
       <c r="C215" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="E215" s="6">
         <v>60</v>
@@ -7421,7 +7408,7 @@
         <v>124</v>
       </c>
       <c r="C216" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="E216" s="6">
         <v>50</v>
@@ -7434,13 +7421,13 @@
     </row>
     <row r="217" spans="1:9" ht="12.75" customHeight="1">
       <c r="A217" s="35" t="s">
+        <v>511</v>
+      </c>
+      <c r="B217" s="12" t="s">
         <v>512</v>
       </c>
-      <c r="B217" s="12" t="s">
-        <v>513</v>
-      </c>
       <c r="C217" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D217" s="12"/>
       <c r="G217" s="4"/>
@@ -7455,7 +7442,7 @@
         <v>72</v>
       </c>
       <c r="C218" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D218" s="12"/>
       <c r="E218" s="10"/>
@@ -7469,10 +7456,10 @@
         <v>243</v>
       </c>
       <c r="B219" s="12" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="C219" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D219" s="12"/>
       <c r="E219" s="10"/>
@@ -7489,7 +7476,7 @@
         <v>293</v>
       </c>
       <c r="C220" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D220" s="12"/>
       <c r="E220" s="10"/>
@@ -7502,7 +7489,7 @@
     </row>
     <row r="221" spans="1:9" ht="12.75" customHeight="1">
       <c r="C221" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="G221" s="4"/>
       <c r="H221" s="6"/>
@@ -7512,9 +7499,6 @@
       <c r="A222" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="C222" s="4" t="s">
-        <v>608</v>
-      </c>
       <c r="G222" s="4"/>
       <c r="H222" s="6"/>
       <c r="I222" s="6"/>
@@ -7524,7 +7508,7 @@
         <v>139</v>
       </c>
       <c r="C223" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="E223" s="6">
         <v>25</v>
@@ -7540,7 +7524,7 @@
         <v>140</v>
       </c>
       <c r="C224" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="E224" s="6">
         <v>20</v>
@@ -7556,7 +7540,7 @@
         <v>141</v>
       </c>
       <c r="C225" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="E225" s="6">
         <v>50</v>
@@ -7572,7 +7556,7 @@
         <v>142</v>
       </c>
       <c r="C226" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="E226" s="6">
         <v>50</v>
@@ -7588,7 +7572,7 @@
         <v>143</v>
       </c>
       <c r="C227" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="E227" s="6">
         <v>55</v>
@@ -7604,7 +7588,7 @@
         <v>144</v>
       </c>
       <c r="C228" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="E228" s="6">
         <v>35</v>
@@ -7620,7 +7604,7 @@
         <v>145</v>
       </c>
       <c r="C229" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="E229" s="6">
         <v>40</v>
@@ -7636,7 +7620,7 @@
         <v>146</v>
       </c>
       <c r="C230" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="E230" s="6">
         <v>25</v>
@@ -7652,7 +7636,7 @@
         <v>201</v>
       </c>
       <c r="C231" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="E231" s="6">
         <v>25</v>
@@ -7665,11 +7649,11 @@
     </row>
     <row r="232" spans="1:10" ht="12.75" customHeight="1">
       <c r="A232" s="26" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B232" s="26"/>
       <c r="C232" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D232" s="26"/>
       <c r="E232" s="27">
@@ -7677,18 +7661,18 @@
       </c>
       <c r="F232" s="27"/>
       <c r="G232" s="26" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="H232" s="6"/>
       <c r="I232" s="6"/>
     </row>
     <row r="233" spans="1:10" s="28" customFormat="1" ht="12.75" customHeight="1">
       <c r="A233" s="26" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B233" s="26"/>
       <c r="C233" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D233" s="26"/>
       <c r="E233" s="27">
@@ -7704,11 +7688,11 @@
     </row>
     <row r="234" spans="1:10" ht="12.75" customHeight="1">
       <c r="A234" s="26" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="B234" s="26"/>
       <c r="C234" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D234" s="26"/>
       <c r="E234" s="27">
@@ -7716,18 +7700,18 @@
       </c>
       <c r="F234" s="27"/>
       <c r="G234" s="26" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="H234" s="6"/>
       <c r="I234" s="6"/>
     </row>
     <row r="235" spans="1:10" ht="12.75" customHeight="1">
       <c r="A235" s="26" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B235" s="26"/>
       <c r="C235" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D235" s="26"/>
       <c r="E235" s="27">
@@ -7737,18 +7721,18 @@
         <v>8</v>
       </c>
       <c r="G235" s="26" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="H235" s="6"/>
       <c r="I235" s="6"/>
     </row>
     <row r="236" spans="1:10" ht="12.75" customHeight="1">
       <c r="A236" s="26" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="B236" s="26"/>
       <c r="C236" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D236" s="26"/>
       <c r="E236" s="27">
@@ -7756,14 +7740,14 @@
       </c>
       <c r="F236" s="27"/>
       <c r="G236" s="26" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="H236" s="6"/>
       <c r="I236" s="6"/>
     </row>
     <row r="237" spans="1:10" ht="12.75" customHeight="1">
       <c r="C237" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="G237" s="4"/>
       <c r="H237" s="6"/>
@@ -7774,7 +7758,7 @@
         <v>74</v>
       </c>
       <c r="C238" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="G238" s="4"/>
       <c r="H238" s="6"/>
@@ -7785,7 +7769,7 @@
         <v>194</v>
       </c>
       <c r="C239" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="E239" s="6">
         <v>50</v>
@@ -7801,7 +7785,7 @@
         <v>200</v>
       </c>
       <c r="C240" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="E240" s="6">
         <v>45</v>
@@ -7817,7 +7801,7 @@
         <v>195</v>
       </c>
       <c r="C241" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="E241" s="6">
         <v>40</v>
@@ -7833,7 +7817,7 @@
         <v>219</v>
       </c>
       <c r="C242" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="E242" s="6">
         <v>30</v>
@@ -7849,7 +7833,7 @@
         <v>196</v>
       </c>
       <c r="C243" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="E243" s="6">
         <v>30</v>
@@ -7862,16 +7846,16 @@
     </row>
     <row r="244" spans="1:11" ht="12.75" customHeight="1">
       <c r="A244" s="4" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="C244" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="E244" s="6">
         <v>15</v>
       </c>
       <c r="G244" s="4" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="H244" s="4"/>
       <c r="I244" s="6"/>
@@ -7881,7 +7865,7 @@
         <v>147</v>
       </c>
       <c r="C245" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="E245" s="6">
         <v>35</v>
@@ -7895,7 +7879,7 @@
         <v>148</v>
       </c>
       <c r="C246" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="E246" s="6">
         <v>45</v>
@@ -7906,10 +7890,10 @@
     </row>
     <row r="247" spans="1:11" ht="12.75" customHeight="1">
       <c r="A247" s="4" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="C247" s="4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="E247" s="6">
         <v>25</v>
@@ -7922,7 +7906,7 @@
     </row>
     <row r="248" spans="1:11" s="28" customFormat="1" ht="12.75" customHeight="1">
       <c r="A248" s="26" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B248" s="26" t="s">
         <v>206</v>
@@ -7934,7 +7918,7 @@
       </c>
       <c r="F248" s="27"/>
       <c r="G248" s="26" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="H248" s="26"/>
       <c r="I248" s="27"/>
@@ -7942,7 +7926,7 @@
     </row>
     <row r="249" spans="1:11" s="36" customFormat="1" ht="12.75" customHeight="1">
       <c r="A249" s="26" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="B249" s="26" t="s">
         <v>288</v>
@@ -7956,7 +7940,7 @@
         <v>16</v>
       </c>
       <c r="G249" s="26" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="H249" s="26" t="s">
         <v>289</v>

</xml_diff>